<commit_message>
Rodada 6 - Fase 2
Atualização da Rodada 6 e ajuste da Fase 2 da Libertadores. Ainda falta ajustar a rodada 6 das séries C e D.
</commit_message>
<xml_diff>
--- a/libertadores/datasets_liberta/classificacao_por_grupo_fase2.xlsx
+++ b/libertadores/datasets_liberta/classificacao_por_grupo_fase2.xlsx
@@ -58,61 +58,61 @@
     <t>Grupo I</t>
   </si>
   <si>
+    <t>Dom Camillo68</t>
+  </si>
+  <si>
+    <t>lsauer fc</t>
+  </si>
+  <si>
+    <t>Analove10 ITAQUI GRANDE!!</t>
+  </si>
+  <si>
+    <t>Super Vasco f.c</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>1_A</t>
+  </si>
+  <si>
+    <t>2_B</t>
+  </si>
+  <si>
+    <t>1_C</t>
+  </si>
+  <si>
+    <t>2_D</t>
+  </si>
+  <si>
+    <t>Grupo J</t>
+  </si>
+  <si>
+    <t>Tabajara de Inhaua FC2</t>
+  </si>
+  <si>
     <t>pura bucha /botafogo</t>
   </si>
   <si>
-    <t>lsauer fc</t>
-  </si>
-  <si>
-    <t>Grêmio imortal 37</t>
-  </si>
-  <si>
     <t>Texas Club 2025</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>1_A</t>
-  </si>
-  <si>
-    <t>2_B</t>
-  </si>
-  <si>
-    <t>1_C</t>
-  </si>
-  <si>
-    <t>2_D</t>
-  </si>
-  <si>
-    <t>Grupo J</t>
-  </si>
-  <si>
-    <t>Tabajara de Inhaua FC2</t>
-  </si>
-  <si>
-    <t>Dom Camillo68</t>
-  </si>
-  <si>
-    <t>Tatols Beants F.C</t>
-  </si>
-  <si>
-    <t>Analove10 ITAQUI GRANDE!!</t>
+    <t>TEAM LOPES 99</t>
   </si>
   <si>
     <t>1_B</t>
@@ -133,43 +133,43 @@
     <t>Real SCI</t>
   </si>
   <si>
+    <t>Lá do Itaqui</t>
+  </si>
+  <si>
+    <t>KING LEONN</t>
+  </si>
+  <si>
+    <t>Laranjja Mecannica</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>1_E</t>
+  </si>
+  <si>
+    <t>2_F</t>
+  </si>
+  <si>
+    <t>1_G</t>
+  </si>
+  <si>
+    <t>2_H</t>
+  </si>
+  <si>
+    <t>Grupo L</t>
+  </si>
+  <si>
     <t>TORRESMO COM PINGA</t>
-  </si>
-  <si>
-    <t>KING LEONN</t>
-  </si>
-  <si>
-    <t>Laranjja Mecannica</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>1_E</t>
-  </si>
-  <si>
-    <t>2_F</t>
-  </si>
-  <si>
-    <t>1_G</t>
-  </si>
-  <si>
-    <t>2_H</t>
-  </si>
-  <si>
-    <t>Grupo L</t>
-  </si>
-  <si>
-    <t>Lá do Itaqui</t>
   </si>
   <si>
     <t>Gremiomaniasm</t>
@@ -602,6 +602,24 @@
       <c r="C2">
         <v>12</v>
       </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>520.8798828125</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
       <c r="J2" t="s">
         <v>17</v>
       </c>
@@ -620,7 +638,25 @@
         <v>14</v>
       </c>
       <c r="C3">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>513.55029296875</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
       </c>
       <c r="J3" t="s">
         <v>18</v>
@@ -640,7 +676,25 @@
         <v>15</v>
       </c>
       <c r="C4">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>526.31005859375</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
       </c>
       <c r="J4" t="s">
         <v>17</v>
@@ -661,6 +715,24 @@
       </c>
       <c r="C5">
         <v>9</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>505.749755859375</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
       </c>
       <c r="J5" t="s">
         <v>18</v>
@@ -733,6 +805,24 @@
       <c r="C2">
         <v>12</v>
       </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>522.12060546875</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
       <c r="J2" t="s">
         <v>17</v>
       </c>
@@ -751,7 +841,25 @@
         <v>29</v>
       </c>
       <c r="C3">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>466.9794921875</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
       </c>
       <c r="J3" t="s">
         <v>18</v>
@@ -771,7 +879,25 @@
         <v>30</v>
       </c>
       <c r="C4">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>501.6298828125</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
       </c>
       <c r="J4" t="s">
         <v>17</v>
@@ -792,6 +918,24 @@
       </c>
       <c r="C5">
         <v>9</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>518.08984375</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
       </c>
       <c r="J5" t="s">
         <v>18</v>
@@ -864,6 +1008,24 @@
       <c r="C2">
         <v>15</v>
       </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>552.1396484375</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
       <c r="J2" t="s">
         <v>17</v>
       </c>
@@ -882,7 +1044,25 @@
         <v>38</v>
       </c>
       <c r="C3">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>507.43017578125</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
       </c>
       <c r="J3" t="s">
         <v>18</v>
@@ -902,7 +1082,25 @@
         <v>39</v>
       </c>
       <c r="C4">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>513.68994140625</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
       </c>
       <c r="J4" t="s">
         <v>17</v>
@@ -923,6 +1121,24 @@
       </c>
       <c r="C5">
         <v>12</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>443.39990234375</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
       </c>
       <c r="J5" t="s">
         <v>18</v>
@@ -995,6 +1211,24 @@
       <c r="C2">
         <v>12</v>
       </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>514.140625</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
       <c r="J2" t="s">
         <v>17</v>
       </c>
@@ -1013,7 +1247,25 @@
         <v>51</v>
       </c>
       <c r="C3">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>500.619384765625</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
       </c>
       <c r="J3" t="s">
         <v>18</v>
@@ -1035,6 +1287,24 @@
       <c r="C4">
         <v>12</v>
       </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>504.9794921875</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
       <c r="J4" t="s">
         <v>17</v>
       </c>
@@ -1054,6 +1324,24 @@
       </c>
       <c r="C5">
         <v>9</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>469.429931640625</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
       </c>
       <c r="J5" t="s">
         <v>18</v>

</xml_diff>